<commit_message>
now in total_frame is a sum of done
</commit_message>
<xml_diff>
--- a/months/m23/m23.xlsx
+++ b/months/m23/m23.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="184">
   <si>
     <t xml:space="preserve">DATE</t>
   </si>
@@ -322,9 +322,21 @@
     <t xml:space="preserve">РУГАНЬ</t>
   </si>
   <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150</t>
+  </si>
+  <si>
     <t xml:space="preserve">РАСПРАВА</t>
   </si>
   <si>
+    <t xml:space="preserve">200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
     <t xml:space="preserve">ЧАШКА</t>
   </si>
   <si>
@@ -334,12 +346,18 @@
     <t xml:space="preserve">СОЖАЛЕНИЕ</t>
   </si>
   <si>
+    <t xml:space="preserve">400</t>
+  </si>
+  <si>
     <t xml:space="preserve">В МАСЛЕ</t>
   </si>
   <si>
     <t xml:space="preserve">СТИРКА ПОСЛЕ 21</t>
   </si>
   <si>
+    <t xml:space="preserve">300</t>
+  </si>
+  <si>
     <t xml:space="preserve">ПЫЛЕСОС</t>
   </si>
   <si>
@@ -349,18 +367,21 @@
     <t xml:space="preserve">поощрения</t>
   </si>
   <si>
+    <t xml:space="preserve">250</t>
+  </si>
+  <si>
     <t xml:space="preserve">прививка</t>
   </si>
   <si>
-    <t xml:space="preserve">100</t>
-  </si>
-  <si>
     <t xml:space="preserve">категория</t>
   </si>
   <si>
     <t xml:space="preserve">новая работа</t>
   </si>
   <si>
+    <t xml:space="preserve">-650</t>
+  </si>
+  <si>
     <t xml:space="preserve">category</t>
   </si>
   <si>
@@ -445,7 +466,7 @@
     <t xml:space="preserve">30*</t>
   </si>
   <si>
-    <t xml:space="preserve">{"&lt;.22": "2*", "&lt;.23": "1.5*", "&gt;.23": "-0.5*"}</t>
+    <t xml:space="preserve">{"&lt;.22": "2*", "&lt;=.23": "1.5*", "&gt;.23": "-0.5*"}</t>
   </si>
   <si>
     <t xml:space="preserve">{"1": 25, "2": 0}</t>
@@ -469,7 +490,7 @@
     <t xml:space="preserve">{"+": {"CDIF": 50, "P": 25}, "-": {"CDIF": 0, "P": -25}}</t>
   </si>
   <si>
-    <t xml:space="preserve">{"&lt;.23": "1*", "&gt;.23": 0, "&gt;.0": "-1.5*"}</t>
+    <t xml:space="preserve">{"&lt;=.23": "1*", "&gt;.23": 0, "&gt;.0": "-0.5*"}</t>
   </si>
   <si>
     <t xml:space="preserve">10*</t>
@@ -478,16 +499,13 @@
     <t xml:space="preserve">{"9": 100, "True": 0}</t>
   </si>
   <si>
-    <t xml:space="preserve">{"&lt;.23": "3*", "&gt;.23": 0}</t>
-  </si>
-  <si>
     <t xml:space="preserve">dutyFalse</t>
   </si>
   <si>
     <t xml:space="preserve">True</t>
   </si>
   <si>
-    <t xml:space="preserve">{"&lt;.22": "1.5*", "&lt;.23": "1*", "&gt;.23": "-1*"}</t>
+    <t xml:space="preserve">{"&lt;.22": "1.5*", "&lt;=.23": "1*", "&gt;.23": "-1*"}</t>
   </si>
   <si>
     <t xml:space="preserve">{"1": 25, "2": -25}</t>
@@ -500,6 +518,9 @@
   </si>
   <si>
     <t xml:space="preserve">{"+": {"CDIF": 100, "P": 50}, "-": {"CDIFP": 0}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"&lt;=.23": "1*", "&gt;.23": 0, "&gt;.0": "-1.5*"}</t>
   </si>
   <si>
     <t xml:space="preserve">False</t>
@@ -560,16 +581,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd&quot;, &quot;mmmm\ dd&quot;, &quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="d/m;@"/>
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="General"/>
-    <numFmt numFmtId="169" formatCode="0.00"/>
-    <numFmt numFmtId="170" formatCode="h:mm"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00"/>
+    <numFmt numFmtId="170" formatCode="0.00"/>
+    <numFmt numFmtId="171" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -606,6 +628,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -699,7 +727,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -752,6 +780,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -772,15 +804,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -797,6 +829,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -820,11 +856,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -970,11 +1006,11 @@
   <dimension ref="A1:AH32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="S12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="N17" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="Y31" activeCellId="0" sqref="Y31"/>
+      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3531,7 +3567,9 @@
       </c>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
-      <c r="Q32" s="8"/>
+      <c r="Q32" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="R32" s="7" t="s">
         <v>14</v>
       </c>
@@ -3654,42 +3692,48 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="12.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="3" width="8.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="8.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="E1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="s">
         <v>98</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -3698,10 +3742,16 @@
       <c r="C4" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
+      <c r="D4" s="13" t="s">
         <v>99</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>26</v>
@@ -3709,47 +3759,62 @@
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
-        <v>100</v>
+      <c r="D5" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
-        <v>101</v>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="17" t="s">
+        <v>105</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="s">
-        <v>102</v>
+      <c r="E7" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="s">
-        <v>104</v>
+      <c r="D8" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
-        <v>105</v>
+      <c r="E10" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="17" t="s">
+        <v>111</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>10</v>
@@ -3757,15 +3822,21 @@
       <c r="C11" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>59</v>
@@ -3773,13 +3844,20 @@
       <c r="C13" s="0" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>100</v>
@@ -3787,12 +3865,18 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>111</v>
+        <v>117</v>
+      </c>
+      <c r="D17" s="13" t="n">
+        <v>-400</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3836,140 +3920,140 @@
   <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="W1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topRight" activeCell="X10" activeCellId="0" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="19" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="18" width="40.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="18" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="19" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="18" width="40.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="18" width="18.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="18" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="18" width="5.85"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="18" width="9.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="19" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="18" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="18" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="19" width="24.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="20" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="18" width="45.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="18" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="18" width="35.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="20" style="18" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="19" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="18" width="45.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="18" width="35.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="18" width="5.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="26" style="18" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="40.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="19" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="19" width="40.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="19" width="18.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="19" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="19" width="5.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="19" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="20" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="19" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="19" width="9.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="20" width="24.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="21" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="19" width="45.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="19" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="19" width="35.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="20" style="19" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="20" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="19" width="45.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="19" width="35.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="19" width="5.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="26" style="19" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>113</v>
+      <c r="A1" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>116</v>
+        <v>122</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>123</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>122</v>
+        <v>128</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>129</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>125</v>
+        <v>131</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>132</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="V1" s="22" t="s">
-        <v>133</v>
+        <v>139</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>140</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>139</v>
+      <c r="A2" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>146</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>142</v>
+        <v>148</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>149</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>50</v>
@@ -3980,23 +4064,23 @@
       <c r="J2" s="12" t="n">
         <v>150</v>
       </c>
-      <c r="K2" s="24" t="s">
-        <v>144</v>
+      <c r="K2" s="25" t="s">
+        <v>151</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="M2" s="12" t="n">
         <v>50</v>
       </c>
-      <c r="N2" s="24" t="s">
-        <v>145</v>
+      <c r="N2" s="25" t="s">
+        <v>152</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="Q2" s="12" t="n">
         <v>50</v>
@@ -4004,36 +4088,36 @@
       <c r="R2" s="12" t="n">
         <v>50</v>
       </c>
-      <c r="S2" s="12" t="s">
-        <v>148</v>
+      <c r="S2" s="26" t="s">
+        <v>155</v>
       </c>
       <c r="T2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="V2" s="24" t="s">
-        <v>150</v>
+        <v>156</v>
+      </c>
+      <c r="V2" s="25" t="s">
+        <v>157</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>151</v>
+        <v>154</v>
+      </c>
+      <c r="X2" s="26" t="s">
+        <v>155</v>
       </c>
       <c r="Y2" s="0" t="n">
         <v>50</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" s="24" t="n">
+      <c r="A3" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="25" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="12" t="n">
@@ -4042,7 +4126,7 @@
       <c r="D3" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="24" t="n">
+      <c r="E3" s="25" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="12" t="n">
@@ -4060,14 +4144,14 @@
       <c r="J3" s="12" t="n">
         <v>-25</v>
       </c>
-      <c r="K3" s="24" t="n">
+      <c r="K3" s="25" t="n">
         <v>0</v>
       </c>
       <c r="L3" s="12"/>
       <c r="M3" s="12" t="n">
         <v>-50</v>
       </c>
-      <c r="N3" s="24" t="n">
+      <c r="N3" s="25" t="n">
         <v>-50</v>
       </c>
       <c r="O3" s="12" t="n">
@@ -4091,7 +4175,7 @@
       <c r="U3" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="V3" s="24" t="n">
+      <c r="V3" s="25" t="n">
         <v>0</v>
       </c>
       <c r="W3" s="12" t="n">
@@ -4108,26 +4192,26 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>146</v>
-      </c>
       <c r="C4" s="12" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>142</v>
+        <v>161</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>149</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>0</v>
@@ -4138,23 +4222,23 @@
       <c r="J4" s="12" t="n">
         <v>50</v>
       </c>
-      <c r="K4" s="24" t="s">
-        <v>146</v>
+      <c r="K4" s="25" t="s">
+        <v>153</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="M4" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="N4" s="24" t="s">
-        <v>157</v>
+      <c r="N4" s="25" t="s">
+        <v>163</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="Q4" s="12" t="n">
         <v>100</v>
@@ -4163,35 +4247,35 @@
         <v>100</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="T4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="V4" s="24" t="s">
-        <v>157</v>
+        <v>153</v>
+      </c>
+      <c r="V4" s="25" t="s">
+        <v>163</v>
       </c>
       <c r="W4" s="12" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="X4" s="12" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="Y4" s="0" t="n">
         <v>50</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="B5" s="24" t="n">
+      <c r="A5" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="25" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="12" t="n">
@@ -4200,7 +4284,7 @@
       <c r="D5" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="24" t="n">
+      <c r="E5" s="25" t="n">
         <v>-50</v>
       </c>
       <c r="F5" s="12" t="n">
@@ -4218,14 +4302,14 @@
       <c r="J5" s="12" t="n">
         <v>-50</v>
       </c>
-      <c r="K5" s="24" t="n">
+      <c r="K5" s="25" t="n">
         <v>0</v>
       </c>
       <c r="L5" s="12"/>
       <c r="M5" s="12" t="n">
         <v>-50</v>
       </c>
-      <c r="N5" s="24" t="n">
+      <c r="N5" s="25" t="n">
         <v>-50</v>
       </c>
       <c r="O5" s="12"/>
@@ -4247,7 +4331,7 @@
       <c r="U5" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="V5" s="24" t="n">
+      <c r="V5" s="25" t="n">
         <v>-50</v>
       </c>
       <c r="W5" s="12" t="n">
@@ -4264,7 +4348,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="28" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="9" t="n">
@@ -4304,28 +4388,28 @@
         <v>1</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="O6" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="V6" s="9" t="n">
         <v>1</v>
@@ -4344,8 +4428,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
-        <v>161</v>
+      <c r="A7" s="29" t="s">
+        <v>168</v>
       </c>
       <c r="B7" s="9" t="n">
         <v>0.75</v>
@@ -4424,8 +4508,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="28" t="s">
-        <v>162</v>
+      <c r="A8" s="30" t="s">
+        <v>169</v>
       </c>
       <c r="B8" s="9" t="n">
         <v>1.25</v>
@@ -4504,8 +4588,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="28" t="s">
-        <v>163</v>
+      <c r="A9" s="30" t="s">
+        <v>170</v>
       </c>
       <c r="B9" s="9" t="n">
         <v>1.5</v>
@@ -4584,7 +4668,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="9" t="n">
@@ -4664,7 +4748,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="31" t="s">
         <v>46</v>
       </c>
       <c r="B11" s="9" t="n">
@@ -4744,194 +4828,194 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30" t="s">
-        <v>164</v>
-      </c>
-      <c r="B12" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="18" t="n">
+      <c r="A12" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="19" t="n">
         <v>0.5</v>
       </c>
-      <c r="K12" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="M12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="N12" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="O12" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="P12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="R12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="S12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="T12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="U12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="V12" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="W12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="X12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y12" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z12" s="18" t="n">
+      <c r="K12" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="P12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="R12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="S12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="T12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="U12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="V12" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="W12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="X12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="19" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="18" t="n">
+      <c r="B13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="19" t="n">
         <v>0.5</v>
       </c>
-      <c r="K13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="M13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="N13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="O13" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="P13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="R13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="S13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="T13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="U13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="V13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="W13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="X13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y13" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z13" s="18" t="n">
+      <c r="K13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="P13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="R13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="S13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="T13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="U13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="V13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="W13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="X13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="19" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I16" s="20"/>
+      <c r="I16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I17" s="20"/>
+      <c r="I17" s="21"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I18" s="20"/>
+      <c r="I18" s="21"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I19" s="20"/>
+      <c r="I19" s="21"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I20" s="20"/>
+      <c r="I20" s="21"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I21" s="20"/>
+      <c r="I21" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I22" s="20"/>
+      <c r="I22" s="21"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I23" s="20"/>
+      <c r="I23" s="21"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I24" s="20"/>
+      <c r="I24" s="21"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I25" s="20"/>
+      <c r="I25" s="21"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:AMJ13">
@@ -4988,7 +5072,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>3</v>
@@ -5116,16 +5200,16 @@
         <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="G2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>10</v>
@@ -5134,7 +5218,7 @@
         <v>10</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>13</v>
@@ -5164,7 +5248,7 @@
         <v>13</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>13</v>
@@ -5176,7 +5260,7 @@
         <v>1</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="Z2" s="0" t="n">
         <v>1</v>
@@ -5202,16 +5286,16 @@
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="G3" s="3" t="n">
         <v>2</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>26</v>
@@ -5220,13 +5304,13 @@
         <v>26</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="W3" s="3" t="n">
         <v>2</v>
@@ -5235,7 +5319,7 @@
         <v>2</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="Z3" s="0" t="n">
         <v>2</v>
@@ -5249,31 +5333,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="W4" s="3" t="n">
         <v>3</v>
@@ -5282,7 +5366,7 @@
         <v>3</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="Z4" s="0" t="n">
         <v>3</v>
@@ -5296,31 +5380,31 @@
         <v>4</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>43</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="W5" s="3" t="n">
         <v>4</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="AB5" s="3" t="n">
         <v>4</v>
@@ -5331,28 +5415,28 @@
         <v>5</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>59</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>59</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5361,61 +5445,61 @@
       </c>
       <c r="F7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="31"/>
-      <c r="H8" s="31"/>
+      <c r="F8" s="33"/>
+      <c r="H8" s="33"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="F9" s="33"/>
+      <c r="H9" s="33"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="31"/>
-      <c r="H10" s="31"/>
+      <c r="F10" s="33"/>
+      <c r="H10" s="33"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="31"/>
-      <c r="H11" s="31"/>
+      <c r="F11" s="33"/>
+      <c r="H11" s="33"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="31"/>
-      <c r="H12" s="31"/>
+      <c r="F12" s="33"/>
+      <c r="H12" s="33"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F13" s="31"/>
-      <c r="H13" s="31"/>
+      <c r="F13" s="33"/>
+      <c r="H13" s="33"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="31"/>
-      <c r="H14" s="31"/>
+      <c r="F14" s="33"/>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="F15" s="33"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="31"/>
-      <c r="H16" s="31"/>
+      <c r="F16" s="33"/>
+      <c r="H16" s="33"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="F17" s="33"/>
+      <c r="H17" s="33"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="31"/>
-      <c r="H18" s="31"/>
+      <c r="F18" s="33"/>
+      <c r="H18" s="33"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>